<commit_message>
Updated hours sheet 2/21
</commit_message>
<xml_diff>
--- a/Hours Sheet.xlsx
+++ b/Hours Sheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabekrishnadasan/Desktop/VentureX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B5A6E5-9F56-654D-AA8D-D5DC91A9421D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C82F00-12A4-FA4B-A159-F3C02305B76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{464AAE45-CF7A-9649-A32F-CC318227CD4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -394,44 +397,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F140423-B78F-214D-A162-D84E78E9A92E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>45294</v>
+        <v>45325</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <f>SUM(B2:B30)</f>
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>45296</v>
+        <v>45327</v>
       </c>
       <c r="B3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>45304</v>
+        <v>45335</v>
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45343</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>